<commit_message>
lot's of minor changes
</commit_message>
<xml_diff>
--- a/data/cas_attribute_values.xlsx
+++ b/data/cas_attribute_values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20346"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20348"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PIVER37\Documents\github\cas\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PIVER37\Documents\casfri\cas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A13C8919-21CB-47DB-A5EE-296EADA5AA20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3397BD38-A653-441A-8385-A789C189A6A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="5540" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="5540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HDR" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="155">
   <si>
     <t>Attribute</t>
   </si>
@@ -456,31 +456,56 @@
     <t>FIP, I, VRI</t>
   </si>
   <si>
-    <t>Jurisdiction</t>
-  </si>
-  <si>
-    <t>BC08</t>
-  </si>
-  <si>
-    <t>AB06, AB16</t>
-  </si>
-  <si>
-    <t>NB01</t>
-  </si>
-  <si>
-    <t>AB16</t>
-  </si>
-  <si>
-    <t>AB06</t>
+    <t>ORIG_STAND_ID</t>
+  </si>
+  <si>
+    <t>STAND_STRUCTURE</t>
+  </si>
+  <si>
+    <t>NUM_OF_LAYERS</t>
+  </si>
+  <si>
+    <t>IDENTIFICATION_ID</t>
+  </si>
+  <si>
+    <t>MAP_SHEET_ID</t>
+  </si>
+  <si>
+    <t>GIS_AREA</t>
+  </si>
+  <si>
+    <t>GIS_PERIMETER</t>
+  </si>
+  <si>
+    <t>INVENTORY_AREA</t>
+  </si>
+  <si>
+    <t>PHOTO_YEAR</t>
+  </si>
+  <si>
+    <t>AB01</t>
+  </si>
+  <si>
+    <t>Alphanumeric code consisting of jurisdiction and inventory version</t>
+  </si>
+  <si>
+    <t>1-9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -934,53 +959,54 @@
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1335,426 +1361,254 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.453125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>143</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B5" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B6" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="2" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B8" s="2" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B9" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="2" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B10" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="2" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="2" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B13" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="2" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B14" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B14" s="2" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B15" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B15" s="2" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B16" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C16" s="2" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B24" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="B25" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="B29" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B31" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B32" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" s="2" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1765,28 +1619,131 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="45.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.81640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="186.81640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1794,10 +1751,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1816,10 +1773,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1827,10 +1784,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1838,10 +1795,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1849,10 +1806,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1860,10 +1817,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1871,32 +1828,32 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" s="3">
-        <v>43474</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" s="3">
-        <v>43474</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1904,21 +1861,21 @@
         <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C12" s="3">
-        <v>43474</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1926,21 +1883,21 @@
         <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>27</v>
+      <c r="A14" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -1948,10 +1905,10 @@
         <v>27</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1959,10 +1916,10 @@
         <v>27</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1970,10 +1927,10 @@
         <v>31</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1981,10 +1938,10 @@
         <v>31</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1992,10 +1949,10 @@
         <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -2003,10 +1960,10 @@
         <v>34</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -2014,10 +1971,10 @@
         <v>34</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -2025,10 +1982,10 @@
         <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -2036,10 +1993,10 @@
         <v>34</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -2047,10 +2004,10 @@
         <v>34</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -2058,10 +2015,10 @@
         <v>34</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -2069,10 +2026,10 @@
         <v>34</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -2080,10 +2037,10 @@
         <v>49</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -2091,10 +2048,10 @@
         <v>52</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -2102,10 +2059,10 @@
         <v>54</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -2113,10 +2070,10 @@
         <v>54</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -2124,10 +2081,10 @@
         <v>58</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -2135,10 +2092,10 @@
         <v>58</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -2146,10 +2103,10 @@
         <v>58</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -2157,10 +2114,10 @@
         <v>58</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -2168,10 +2125,10 @@
         <v>58</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -2179,10 +2136,10 @@
         <v>65</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2191,10 +2148,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2203,7 +2162,7 @@
     <col min="3" max="3" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2214,124 +2173,138 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2341,10 +2314,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2366,18 +2341,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>76</v>
+        <v>138</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>139</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -2388,7 +2363,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -2399,7 +2374,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -2410,7 +2385,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
@@ -2421,7 +2396,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
@@ -2432,7 +2407,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
@@ -2443,7 +2418,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
@@ -2454,7 +2429,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>3</v>
@@ -2465,7 +2440,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>3</v>
@@ -2476,7 +2451,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>3</v>
@@ -2487,7 +2462,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>3</v>
@@ -2498,12 +2473,23 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2513,10 +2499,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2538,18 +2526,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>139</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -2560,7 +2548,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -2571,7 +2559,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -2582,12 +2570,23 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>